<commit_message>
Fix Render deployment: add apt-packages, update requirements, configure headless Chrome
</commit_message>
<xml_diff>
--- a/extracted_bills_data.xlsx
+++ b/extracted_bills_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>FILE_NAME</t>
   </si>
@@ -73,94 +73,49 @@
     <t>FILE_PATH</t>
   </si>
   <si>
-    <t>FESCO_28131515101100.pdf</t>
-  </si>
-  <si>
-    <t>FESCO_24135425600600.pdf</t>
-  </si>
-  <si>
-    <t>FESCO</t>
-  </si>
-  <si>
-    <t>28131515101100</t>
-  </si>
-  <si>
-    <t>24135425600600</t>
-  </si>
-  <si>
-    <t>19989941998994</t>
-  </si>
-  <si>
-    <t>505</t>
-  </si>
-  <si>
-    <t>212</t>
-  </si>
-  <si>
-    <t>219</t>
+    <t>GEPCO_30123630360500.pdf</t>
+  </si>
+  <si>
+    <t>GEPCO</t>
+  </si>
+  <si>
+    <t>30123630360500</t>
+  </si>
+  <si>
+    <t>800</t>
   </si>
   <si>
     <t>A-2c(06)T</t>
   </si>
   <si>
-    <t>B2b(12)T</t>
-  </si>
-  <si>
     <t>AUG-2025</t>
   </si>
   <si>
-    <t>1875600</t>
-  </si>
-  <si>
-    <t>724763</t>
-  </si>
-  <si>
-    <t>3520</t>
-  </si>
-  <si>
-    <t>1514</t>
-  </si>
-  <si>
-    <t>29650</t>
-  </si>
-  <si>
-    <t>13675</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>121</t>
-  </si>
-  <si>
-    <t>1720</t>
-  </si>
-  <si>
-    <t>3582</t>
-  </si>
-  <si>
-    <t>151</t>
-  </si>
-  <si>
-    <t>114</t>
+    <t>1552419</t>
+  </si>
+  <si>
+    <t>2570</t>
+  </si>
+  <si>
+    <t>21760</t>
+  </si>
+  <si>
+    <t>320</t>
+  </si>
+  <si>
+    <t>3480</t>
+  </si>
+  <si>
+    <t>222</t>
   </si>
   <si>
     <t>35.1500</t>
   </si>
   <si>
-    <t>27.4100</t>
-  </si>
-  <si>
     <t>43.8200</t>
   </si>
   <si>
-    <t>36.6800</t>
-  </si>
-  <si>
-    <t>D:\BILLs App\BillWebApp\BillWebApp\downloads\FESCO_28131515101100.pdf</t>
-  </si>
-  <si>
-    <t>D:\BILLs App\BillWebApp\BillWebApp\downloads\FESCO_24135425600600.pdf</t>
+    <t>D:\BILLs App\BillWebApp\BillWebApp\downloads\GEPCO_30123630360500.pdf</t>
   </si>
 </sst>
 </file>
@@ -518,7 +473,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:S3"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -588,111 +543,55 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>25</v>
       </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" t="s">
         <v>28</v>
       </c>
-      <c r="H2" t="s">
+      <c r="M2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" t="s">
         <v>30</v>
       </c>
-      <c r="I2" t="s">
+      <c r="O2" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" t="s">
         <v>31</v>
       </c>
-      <c r="J2" t="s">
+      <c r="R2" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" t="s">
         <v>33</v>
-      </c>
-      <c r="K2" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N2" t="s">
-        <v>41</v>
-      </c>
-      <c r="O2" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>43</v>
-      </c>
-      <c r="R2" t="s">
-        <v>45</v>
-      </c>
-      <c r="S2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N3" t="s">
-        <v>42</v>
-      </c>
-      <c r="O3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>44</v>
-      </c>
-      <c r="R3" t="s">
-        <v>46</v>
-      </c>
-      <c r="S3" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>